<commit_message>
update generator linear examples
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Leader_Expr</t>
   </si>
@@ -66,82 +66,79 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>-0.7216266850368602y_1 + 0.39477388017775145y_2</t>
-  </si>
-  <si>
-    <t>-1.7912731062676341</t>
+    <t>-0.5521679010310857y_1 + 1.3022014575517853y_2</t>
+  </si>
+  <si>
+    <t>0.178833001141403</t>
+  </si>
+  <si>
+    <t>J_0_L0_v</t>
+  </si>
+  <si>
+    <t>0.24011722556595838</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.9514886319980479</t>
+  </si>
+  <si>
+    <t>-4 + 0.8942385335728744y_1 - 0.3075320774265825y_2</t>
+  </si>
+  <si>
+    <t>-0.48451740998464043</t>
+  </si>
+  <si>
+    <t>0.1083236165390392</t>
+  </si>
+  <si>
+    <t>0.8676051265519084</t>
+  </si>
+  <si>
+    <t>-16 - 2x + 4.521646436843442y_1 - 1.3909514494422142y_2</t>
+  </si>
+  <si>
+    <t>-9.62840831252262</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
   </si>
   <si>
-    <t>0.668826785333615</t>
-  </si>
-  <si>
-    <t>0.45431458518070245</t>
-  </si>
-  <si>
-    <t>0.8218084309941561</t>
-  </si>
-  <si>
-    <t>-4 + 0.7216266850368602y_1 - 0.39477388017775145y_2</t>
-  </si>
-  <si>
-    <t>-2.208726893732366</t>
-  </si>
-  <si>
-    <t>0.35490416055703744</t>
-  </si>
-  <si>
-    <t>0.10178942102153064</t>
-  </si>
-  <si>
-    <t>0.31680062490037586</t>
-  </si>
-  <si>
-    <t>-16 - 2x + 3.608133425184301y_1 - 1.9738694008887574y_2</t>
-  </si>
-  <si>
-    <t>-17.817618199605413</t>
-  </si>
-  <si>
-    <t>0.2579054977982502</t>
-  </si>
-  <si>
-    <t>0.017673204237491406</t>
-  </si>
-  <si>
-    <t>0.3206445811758578</t>
-  </si>
-  <si>
-    <t>-48 + 8x + 0.7216266850368602y_1 - 0.39477388017775145y_2</t>
-  </si>
-  <si>
-    <t>-3.112791969958022</t>
-  </si>
-  <si>
-    <t>0.37312343383402724</t>
-  </si>
-  <si>
-    <t>0.7122051554927713</t>
-  </si>
-  <si>
-    <t>0.306789613492331</t>
-  </si>
-  <si>
-    <t>12 - 2x - 1.4432533700737205y_1 + 0.7895477603555029y_2</t>
-  </si>
-  <si>
-    <t>-2.3565299434788542</t>
-  </si>
-  <si>
-    <t>0.9717867614749729</t>
-  </si>
-  <si>
-    <t>0.3910716398908155</t>
-  </si>
-  <si>
-    <t>0.9536156378735784</t>
+    <t>0.1102758390135593</t>
+  </si>
+  <si>
+    <t>0.354493360729913</t>
+  </si>
+  <si>
+    <t>-48 + 8x + 0.7320173915388171y_1 - 0.7792370045384016y_2</t>
+  </si>
+  <si>
+    <t>0.7663766583793723</t>
+  </si>
+  <si>
+    <t>J_Ne_L0_v</t>
+  </si>
+  <si>
+    <t>0.3168885247170169</t>
+  </si>
+  <si>
+    <t>-0.6544593846769445</t>
+  </si>
+  <si>
+    <t>-0.4512271964658938</t>
+  </si>
+  <si>
+    <t>12 - 2x - 1.7884770671457488y_1 + 0.615064154853165y_2</t>
+  </si>
+  <si>
+    <t>-6.781680179888415</t>
+  </si>
+  <si>
+    <t>0.4167665579899481</t>
+  </si>
+  <si>
+    <t>0.43944029502068416</t>
   </si>
   <si>
     <t>x</t>
@@ -153,34 +150,34 @@
     <t>y_2</t>
   </si>
   <si>
-    <t>5.386991865471793</t>
-  </si>
-  <si>
-    <t>4.081261346001524</t>
-  </si>
-  <si>
-    <t>2.9228731878030403</t>
+    <t>5.875357499928848</t>
+  </si>
+  <si>
+    <t>4.657691821664619</t>
+  </si>
+  <si>
+    <t>2.112315956957238</t>
   </si>
   <si>
     <t>vec_bf</t>
   </si>
   <si>
-    <t>1.429256187755491</t>
-  </si>
-  <si>
-    <t>-0.23482935753947165</t>
+    <t>1.0504990379377572</t>
+  </si>
+  <si>
+    <t>-0.13538658216037253</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>-3.880151555685557</t>
-  </si>
-  <si>
-    <t>3.241093503453122</t>
-  </si>
-  <si>
-    <t>-2.13189287455324</t>
+    <t>7.114555667456925</t>
+  </si>
+  <si>
+    <t>3.4891586055754855</t>
+  </si>
+  <si>
+    <t>-2.5134465372185693</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -654,38 +651,38 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -705,7 +702,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -714,7 +711,7 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -732,24 +729,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -767,17 +764,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -795,22 +792,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -828,17 +825,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.483050845102423</v>
+        <v>0.29418144510420585</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.6850364104385369</v>
+        <v>0.8554177056119834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add almost all lineal
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Leader_Expr</t>
   </si>
@@ -66,79 +66,82 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>-0.5521679010310857y_1 + 1.3022014575517853y_2</t>
-  </si>
-  <si>
-    <t>0.178833001141403</t>
+    <t>-0.9446013643891683y_1 + 0.011004345402239183y_2</t>
+  </si>
+  <si>
+    <t>-4.113656050722677</t>
   </si>
   <si>
     <t>J_0_L0_v</t>
   </si>
   <si>
-    <t>0.24011722556595838</t>
+    <t>0.0866877650392671</t>
+  </si>
+  <si>
+    <t>-0.2704755559527997</t>
+  </si>
+  <si>
+    <t>-0.4724490455978724</t>
+  </si>
+  <si>
+    <t>-4 + 1.4258984934749632y_1 + 0.08460017249189158y_2</t>
+  </si>
+  <si>
+    <t>2.4513323248895706</t>
+  </si>
+  <si>
+    <t>0.9648587319705634</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>0.9514886319980479</t>
-  </si>
-  <si>
-    <t>-4 + 0.8942385335728744y_1 - 0.3075320774265825y_2</t>
-  </si>
-  <si>
-    <t>-0.48451740998464043</t>
-  </si>
-  <si>
-    <t>0.1083236165390392</t>
-  </si>
-  <si>
-    <t>0.8676051265519084</t>
-  </si>
-  <si>
-    <t>-16 - 2x + 4.521646436843442y_1 - 1.3909514494422142y_2</t>
-  </si>
-  <si>
-    <t>-9.62840831252262</t>
+    <t>0.7232519754967422</t>
+  </si>
+  <si>
+    <t>-16 - 2x + 0.11759800913107077y_1 + 3.8247202989012488y_2</t>
+  </si>
+  <si>
+    <t>-18.10373805947259</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
   </si>
   <si>
-    <t>0.1102758390135593</t>
-  </si>
-  <si>
-    <t>0.354493360729913</t>
-  </si>
-  <si>
-    <t>-48 + 8x + 0.7320173915388171y_1 - 0.7792370045384016y_2</t>
-  </si>
-  <si>
-    <t>0.7663766583793723</t>
+    <t>0.9761226555169311</t>
+  </si>
+  <si>
+    <t>0.4765093561492265</t>
+  </si>
+  <si>
+    <t>-48 + 8x + 1.9304529951548228y_1 + 0.18482451826358154y_2</t>
+  </si>
+  <si>
+    <t>7.908693258692484</t>
   </si>
   <si>
     <t>J_Ne_L0_v</t>
   </si>
   <si>
-    <t>0.3168885247170169</t>
-  </si>
-  <si>
-    <t>-0.6544593846769445</t>
-  </si>
-  <si>
-    <t>-0.4512271964658938</t>
-  </si>
-  <si>
-    <t>12 - 2x - 1.7884770671457488y_1 + 0.615064154853165y_2</t>
-  </si>
-  <si>
-    <t>-6.781680179888415</t>
-  </si>
-  <si>
-    <t>0.4167665579899481</t>
-  </si>
-  <si>
-    <t>0.43944029502068416</t>
+    <t>0.8143958706897286</t>
+  </si>
+  <si>
+    <t>0.9523557914603366</t>
+  </si>
+  <si>
+    <t>0.9861742737355413</t>
+  </si>
+  <si>
+    <t>12 - 2x + 0.8716114642162638y_1 + 0.5704148498394974y_2</t>
+  </si>
+  <si>
+    <t>5.430374185532117</t>
+  </si>
+  <si>
+    <t>0.23927405565041526</t>
+  </si>
+  <si>
+    <t>0.49375642524538843</t>
   </si>
   <si>
     <t>x</t>
@@ -150,34 +153,34 @@
     <t>y_2</t>
   </si>
   <si>
-    <t>5.875357499928848</t>
-  </si>
-  <si>
-    <t>4.657691821664619</t>
-  </si>
-  <si>
-    <t>2.112315956957238</t>
+    <t>5.875840352759835</t>
+  </si>
+  <si>
+    <t>4.382729079133727</t>
+  </si>
+  <si>
+    <t>2.387767396848251</t>
   </si>
   <si>
     <t>vec_bf</t>
   </si>
   <si>
-    <t>1.0504990379377572</t>
-  </si>
-  <si>
-    <t>-0.13538658216037253</t>
+    <t>-2.189402269966704</t>
+  </si>
+  <si>
+    <t>-4.1029830910370535</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>7.114555667456925</t>
-  </si>
-  <si>
-    <t>3.4891586055754855</t>
-  </si>
-  <si>
-    <t>-2.5134465372185693</t>
+    <t>-5.665827619384239</t>
+  </si>
+  <si>
+    <t>0.8499937791199406</t>
+  </si>
+  <si>
+    <t>-3.9955573010119325</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -651,67 +654,67 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -729,24 +732,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -764,17 +767,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -792,22 +795,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -825,17 +828,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.29418144510420585</v>
+        <v>0.5013171590436929</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.8554177056119834</v>
+        <v>0.09958128234312402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expermits todos no convexos menos el 5to
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -66,82 +66,82 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>-0.9446013643891683y_1 + 0.011004345402239183y_2</t>
-  </si>
-  <si>
-    <t>-4.113656050722677</t>
+    <t>4.366913451651778 - 0.7574285534004321y_1 + 0.4286380056576421y_2</t>
+  </si>
+  <si>
+    <t>-4.366913451651778</t>
   </si>
   <si>
     <t>J_0_L0_v</t>
   </si>
   <si>
-    <t>0.0866877650392671</t>
-  </si>
-  <si>
-    <t>-0.2704755559527997</t>
-  </si>
-  <si>
-    <t>-0.4724490455978724</t>
-  </si>
-  <si>
-    <t>-4 + 1.4258984934749632y_1 + 0.08460017249189158y_2</t>
-  </si>
-  <si>
-    <t>2.4513323248895706</t>
-  </si>
-  <si>
-    <t>0.9648587319705634</t>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>3.3000000000000003</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>0.7232519754967422</t>
-  </si>
-  <si>
-    <t>-16 - 2x + 0.11759800913107077y_1 + 3.8247202989012488y_2</t>
-  </si>
-  <si>
-    <t>-18.10373805947259</t>
+    <t>3.303086074127693 + 0.13373800663553037y_1 - 1.5307358653210148y_2</t>
+  </si>
+  <si>
+    <t>-7.303086074127693</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>-0.8</t>
+  </si>
+  <si>
+    <t>-0.5</t>
+  </si>
+  <si>
+    <t>5.75309525256657 - 2x + 0.22725019028865578y_1 + 2.634505660289932y_2</t>
+  </si>
+  <si>
+    <t>-21.75309525256657</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
   </si>
   <si>
-    <t>0.9761226555169311</t>
-  </si>
-  <si>
-    <t>0.4765093561492265</t>
-  </si>
-  <si>
-    <t>-48 + 8x + 1.9304529951548228y_1 + 0.18482451826358154y_2</t>
-  </si>
-  <si>
-    <t>7.908693258692484</t>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>-64.32691345165179 + 8x + 0.7574285534004321y_1 - 0.4286380056576421y_2</t>
+  </si>
+  <si>
+    <t>15.566913451651782</t>
   </si>
   <si>
     <t>J_Ne_L0_v</t>
   </si>
   <si>
-    <t>0.8143958706897286</t>
-  </si>
-  <si>
-    <t>0.9523557914603366</t>
-  </si>
-  <si>
-    <t>0.9861742737355413</t>
-  </si>
-  <si>
-    <t>12 - 2x + 0.8716114642162638y_1 + 0.5704148498394974y_2</t>
-  </si>
-  <si>
-    <t>5.430374185532117</t>
-  </si>
-  <si>
-    <t>0.23927405565041526</t>
-  </si>
-  <si>
-    <t>0.49375642524538843</t>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>6.602172717320021 - 2x - 1.0159046693889429y_1 + 1.7389542990459823y_2</t>
+  </si>
+  <si>
+    <t>-5.397827282679979</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>0.4</t>
   </si>
   <si>
     <t>x</t>
@@ -153,34 +153,34 @@
     <t>y_2</t>
   </si>
   <si>
-    <t>5.875840352759835</t>
-  </si>
-  <si>
-    <t>4.382729079133727</t>
-  </si>
-  <si>
-    <t>2.387767396848251</t>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>7.35</t>
+  </si>
+  <si>
+    <t>2.8</t>
   </si>
   <si>
     <t>vec_bf</t>
   </si>
   <si>
-    <t>-2.189402269966704</t>
-  </si>
-  <si>
-    <t>-4.1029830910370535</t>
+    <t>1.4594557029431234</t>
+  </si>
+  <si>
+    <t>-1.8783971218584716</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>-5.665827619384239</t>
-  </si>
-  <si>
-    <t>0.8499937791199406</t>
-  </si>
-  <si>
-    <t>-3.9955573010119325</t>
+    <t>-1.6000000000000005</t>
+  </si>
+  <si>
+    <t>7.922637697895098</t>
+  </si>
+  <si>
+    <t>-9.558350631746169</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -671,10 +671,10 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -694,24 +694,24 @@
         <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>36</v>
@@ -833,12 +833,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.5013171590436929</v>
+        <v>0.19446458492740665</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.09958128234312402</v>
+        <v>0.34363035313024864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
volver a generar problemas cuadraticos y lineales
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>Leader_Expr</t>
   </si>
@@ -66,82 +66,85 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>4.366913451651778 - 0.7574285534004321y_1 + 0.4286380056576421y_2</t>
-  </si>
-  <si>
-    <t>-4.366913451651778</t>
+    <t>-2.0847668467443836 - 0.09833191166714061y_1 + 1.105819353615771y_2</t>
+  </si>
+  <si>
+    <t>2.0847668467443836</t>
   </si>
   <si>
     <t>J_0_L0_v</t>
   </si>
   <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>3.3000000000000003</t>
+    <t>0.75</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>3.303086074127693 + 0.13373800663553037y_1 - 1.5307358653210148y_2</t>
-  </si>
-  <si>
-    <t>-7.303086074127693</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>-0.8</t>
-  </si>
-  <si>
-    <t>-0.5</t>
-  </si>
-  <si>
-    <t>5.75309525256657 - 2x + 0.22725019028865578y_1 + 2.634505660289932y_2</t>
-  </si>
-  <si>
-    <t>-21.75309525256657</t>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>5.3586508387830545 - 0.17794521846270506y_1 - 1.444649796227846y_2</t>
+  </si>
+  <si>
+    <t>-9.358650838783054</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>-3.5</t>
+  </si>
+  <si>
+    <t>-3.1</t>
+  </si>
+  <si>
+    <t>65.31672418109892 - 2x - 4.93390077477628y_1 - 3.277425478499212y_2</t>
+  </si>
+  <si>
+    <t>-81.31672418109892</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
   </si>
   <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>-64.32691345165179 + 8x + 0.7574285534004321y_1 - 0.4286380056576421y_2</t>
-  </si>
-  <si>
-    <t>15.566913451651782</t>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>9.8</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>-61.25774950241683 + 8x + 0.6006539664486779y_1 - 0.4897640034119989y_2</t>
+  </si>
+  <si>
+    <t>12.66774950241683</t>
   </si>
   <si>
     <t>J_Ne_L0_v</t>
   </si>
   <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>6.602172717320021 - 2x - 1.0159046693889429y_1 + 1.7389542990459823y_2</t>
-  </si>
-  <si>
-    <t>-5.397827282679979</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>0.4</t>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>-27.698080750639754 - 2x - 3.7129182068050426y_1 - 2.1007487441948633y_2</t>
+  </si>
+  <si>
+    <t>-39.698080750639754</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>-3.5999999999999996</t>
+  </si>
+  <si>
+    <t>-10.0</t>
   </si>
   <si>
     <t>x</t>
@@ -153,34 +156,34 @@
     <t>y_2</t>
   </si>
   <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>7.35</t>
-  </si>
-  <si>
-    <t>2.8</t>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>8.600000000000001</t>
+  </si>
+  <si>
+    <t>2.65</t>
   </si>
   <si>
     <t>vec_bf</t>
   </si>
   <si>
-    <t>1.4594557029431234</t>
-  </si>
-  <si>
-    <t>-1.8783971218584716</t>
+    <t>4.783685991651928</t>
+  </si>
+  <si>
+    <t>2.4048979142900997</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>-1.6000000000000005</t>
-  </si>
-  <si>
-    <t>7.922637697895098</t>
-  </si>
-  <si>
-    <t>-9.558350631746169</t>
+    <t>-63.39999999999999</t>
+  </si>
+  <si>
+    <t>31.596635705782617</t>
+  </si>
+  <si>
+    <t>22.2015343561485</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -671,50 +674,50 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -732,24 +735,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -767,17 +770,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -795,22 +798,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -828,17 +831,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.19446458492740665</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.34363035313024864</v>
+        <v>1.9500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevos experimentos no convexos
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/linear/ex9.1.1/Experimentos_Generador/(ex9.1.1(Linear))__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Leader_Expr</t>
   </si>
@@ -66,85 +66,61 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>-2.0847668467443836 - 0.09833191166714061y_1 + 1.105819353615771y_2</t>
-  </si>
-  <si>
-    <t>2.0847668467443836</t>
+    <t>1.4164683088845837 - 0.4882369222252976y_1 + 0.49986161084970937y_2</t>
+  </si>
+  <si>
+    <t>-1.4164683088845837</t>
   </si>
   <si>
     <t>J_0_L0_v</t>
   </si>
   <si>
-    <t>0.75</t>
+    <t>0.35</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>5.3586508387830545 - 0.17794521846270506y_1 - 1.444649796227846y_2</t>
-  </si>
-  <si>
-    <t>-9.358650838783054</t>
-  </si>
-  <si>
-    <t>0.19</t>
-  </si>
-  <si>
-    <t>-3.5</t>
-  </si>
-  <si>
-    <t>-3.1</t>
-  </si>
-  <si>
-    <t>65.31672418109892 - 2x - 4.93390077477628y_1 - 3.277425478499212y_2</t>
-  </si>
-  <si>
-    <t>-81.31672418109892</t>
+    <t>-1.4164683088845837 + 0.4882369222252976y_1 - 0.49986161084970937y_2</t>
+  </si>
+  <si>
+    <t>-2.5835316911154163</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>20.584306670357044 - 2x - 1.51120952117354y_1 + 1.5471907002491005y_2</t>
+  </si>
+  <si>
+    <t>-36.584306670357044</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
   </si>
   <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>9.8</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>-61.25774950241683 + 8x + 0.6006539664486779y_1 - 0.4897640034119989y_2</t>
-  </si>
-  <si>
-    <t>12.66774950241683</t>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>-67.01646830888458 + 8x + 0.4882369222252976y_1 - 0.49986161084970937y_2</t>
+  </si>
+  <si>
+    <t>18.21646830888458</t>
   </si>
   <si>
     <t>J_Ne_L0_v</t>
   </si>
   <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
-    <t>-27.698080750639754 - 2x - 3.7129182068050426y_1 - 2.1007487441948633y_2</t>
-  </si>
-  <si>
-    <t>-39.698080750639754</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>-3.5999999999999996</t>
-  </si>
-  <si>
-    <t>-10.0</t>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>4.967063382230833 - 2x - 0.9764738444505952y_1 + 0.9997232216994187y_2</t>
+  </si>
+  <si>
+    <t>-7.032936617769167</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
   <si>
     <t>x</t>
@@ -156,34 +132,34 @@
     <t>y_2</t>
   </si>
   <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>8.600000000000001</t>
-  </si>
-  <si>
-    <t>2.65</t>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>2.05</t>
   </si>
   <si>
     <t>vec_bf</t>
   </si>
   <si>
-    <t>4.783685991651928</t>
-  </si>
-  <si>
-    <t>2.4048979142900997</t>
+    <t>1.6270357044007748</t>
+  </si>
+  <si>
+    <t>-0.6419651259341269</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>-63.39999999999999</t>
-  </si>
-  <si>
-    <t>31.596635705782617</t>
-  </si>
-  <si>
-    <t>22.2015343561485</t>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>-2.0</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -637,64 +613,64 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -702,22 +678,22 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -735,24 +711,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -770,17 +746,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -798,22 +774,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -831,17 +807,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>1.59</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>1.9500000000000002</v>
+        <v>1.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>